<commit_message>
Adjusted title and RQs as well as replacing the excel file with the updated version
</commit_message>
<xml_diff>
--- a/results/aggregated-results.xlsx
+++ b/results/aggregated-results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="participantrole" sheetId="4" r:id="rId1"/>
@@ -15,7 +15,9 @@
     <sheet name="symptoms" sheetId="8" r:id="rId6"/>
     <sheet name="swquality" sheetId="10" r:id="rId7"/>
     <sheet name="productivity" sheetId="9" r:id="rId8"/>
-    <sheet name="maintsbsdiffdetails" sheetId="1" r:id="rId9"/>
+    <sheet name="maintsbsdiff" sheetId="12" r:id="rId9"/>
+    <sheet name="maintsbsdiffdetails" sheetId="1" r:id="rId10"/>
+    <sheet name="maintsbsdiffreason" sheetId="11" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">symptoms!$L$9:$N$9</definedName>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="112">
   <si>
     <t>Not sure</t>
   </si>
@@ -335,6 +337,33 @@
   <si>
     <t>Hindered</t>
   </si>
+  <si>
+    <t>If no, why is there no difference with these systems?</t>
+  </si>
+  <si>
+    <t>Customer/management did not allow it.</t>
+  </si>
+  <si>
+    <t>Never thought about changing something.</t>
+  </si>
+  <si>
+    <t>Standard approach is sufficient.</t>
+  </si>
+  <si>
+    <t>We did not know what to change.</t>
+  </si>
+  <si>
+    <t>In your projects in general, does the maintainability process or the usage of tools and metrics differ when working on Service- or Microservice-Based Systems as opposed to other systems?</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes, to some degree.</t>
+  </si>
+  <si>
+    <t>Yes, significantly.</t>
+  </si>
 </sst>
 </file>
 
@@ -387,7 +416,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -405,6 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -482,7 +512,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -591,11 +621,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-250788000"/>
-        <c:axId val="-250798336"/>
+        <c:axId val="310485416"/>
+        <c:axId val="310481888"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-250788000"/>
+        <c:axId val="310485416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -635,10 +665,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-250798336"/>
+        <c:crossAx val="310481888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -646,7 +676,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-250798336"/>
+        <c:axId val="310481888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -694,10 +724,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-250788000"/>
+        <c:crossAx val="310485416"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -735,7 +765,615 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>maintsbsdiffdetails!$A$4:$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Process</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Trust in increased maintainability</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Tools</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Metrics</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Not sure</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>maintsbsdiffdetails!$B$4:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="143355696"/>
+        <c:axId val="143352560"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="143355696"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="143352560"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="143352560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="143355696"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000" b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="outEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>maintsbsdiffreason!$A$4:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Never thought about changing something.</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>We did not know what to change.</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Standard approach is sufficient.</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Customer/management did not allow it.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>maintsbsdiffreason!$B$4:$B$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="outEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="468116760"/>
+        <c:axId val="468121856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="468116760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr lang="en-GB" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468121856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="468121856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="468116760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="1000" b="1"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -805,7 +1443,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -890,11 +1528,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1913107104"/>
-        <c:axId val="-1913080992"/>
+        <c:axId val="142287176"/>
+        <c:axId val="142290704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1913107104"/>
+        <c:axId val="142287176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -934,10 +1572,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1913080992"/>
+        <c:crossAx val="142290704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -945,7 +1583,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1913080992"/>
+        <c:axId val="142290704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,10 +1631,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1913107104"/>
+        <c:crossAx val="142287176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1034,7 +1672,7 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1104,7 +1742,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1285,11 +1923,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1914397216"/>
-        <c:axId val="-1914414624"/>
+        <c:axId val="142289920"/>
+        <c:axId val="142286392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1914397216"/>
+        <c:axId val="142289920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1951,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-2700000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1329,10 +1967,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1914414624"/>
+        <c:crossAx val="142286392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1340,7 +1978,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1914414624"/>
+        <c:axId val="142286392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1388,10 +2026,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1914397216"/>
+        <c:crossAx val="142289920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1429,7 +2067,7 @@
       <a:pPr>
         <a:defRPr sz="1300" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1499,7 +2137,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1632,11 +2270,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2049926576"/>
-        <c:axId val="-2049935280"/>
+        <c:axId val="142283256"/>
+        <c:axId val="142287568"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2049926576"/>
+        <c:axId val="142283256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1660,7 +2298,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -1676,10 +2314,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2049935280"/>
+        <c:crossAx val="142287568"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1687,7 +2325,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2049935280"/>
+        <c:axId val="142287568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1735,10 +2373,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2049926576"/>
+        <c:crossAx val="142283256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1776,7 +2414,7 @@
       <a:pPr>
         <a:defRPr sz="1200" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1846,7 +2484,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -1937,11 +2575,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1913066848"/>
-        <c:axId val="-1913061408"/>
+        <c:axId val="142283648"/>
+        <c:axId val="142284040"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1913066848"/>
+        <c:axId val="142283648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1981,10 +2619,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1913061408"/>
+        <c:crossAx val="142284040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1992,7 +2630,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1913061408"/>
+        <c:axId val="142284040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2040,10 +2678,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1913066848"/>
+        <c:crossAx val="142283648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2081,7 +2719,7 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2151,7 +2789,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2290,11 +2928,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2054932304"/>
-        <c:axId val="-2054952432"/>
+        <c:axId val="142285608"/>
+        <c:axId val="142286000"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2054932304"/>
+        <c:axId val="142285608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2334,10 +2972,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054952432"/>
+        <c:crossAx val="142286000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2345,7 +2983,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2054952432"/>
+        <c:axId val="142286000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2393,10 +3031,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2054932304"/>
+        <c:crossAx val="142285608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2434,7 +3072,7 @@
       <a:pPr>
         <a:defRPr sz="1200" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2504,7 +3142,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2595,11 +3233,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1924171840"/>
-        <c:axId val="-1924192512"/>
+        <c:axId val="143357264"/>
+        <c:axId val="143351776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1924171840"/>
+        <c:axId val="143357264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2639,10 +3277,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924192512"/>
+        <c:crossAx val="143351776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2650,7 +3288,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1924192512"/>
+        <c:axId val="143351776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2698,10 +3336,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924171840"/>
+        <c:crossAx val="143357264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2739,7 +3377,7 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2809,7 +3447,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -2900,11 +3538,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1924185440"/>
-        <c:axId val="-1924179456"/>
+        <c:axId val="143350208"/>
+        <c:axId val="143354128"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1924185440"/>
+        <c:axId val="143350208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2944,10 +3582,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924179456"/>
+        <c:crossAx val="143354128"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2955,7 +3593,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1924179456"/>
+        <c:axId val="143354128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3003,10 +3641,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924185440"/>
+        <c:crossAx val="143350208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3044,7 +3682,7 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3116,7 +3754,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="de-DE"/>
+                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="outEnd"/>
@@ -3150,47 +3788,35 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>maintsbsdiffdetails!$A$4:$A$8</c:f>
+              <c:f>maintsbsdiff!$A$4:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>Process</c:v>
+                  <c:v>No</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Trust in increased maintainability</c:v>
+                  <c:v>Yes, to some degree.</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>Tools</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Metrics</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Not sure</c:v>
+                  <c:v>Yes, significantly.</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>maintsbsdiffdetails!$B$4:$B$8</c:f>
+              <c:f>maintsbsdiff!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>11</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3207,11 +3833,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1924195776"/>
-        <c:axId val="-1924171296"/>
+        <c:axId val="475815032"/>
+        <c:axId val="475815424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1924195776"/>
+        <c:axId val="475815032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3235,11 +3861,11 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
-            <a:pPr>
-              <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:pPr algn="ctr">
+              <a:defRPr lang="en-GB" sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -3251,10 +3877,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924171296"/>
+        <c:crossAx val="475815424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3262,7 +3888,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1924171296"/>
+        <c:axId val="475815424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3310,10 +3936,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="de-DE"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1924195776"/>
+        <c:crossAx val="475815032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3351,7 +3977,7 @@
       <a:pPr>
         <a:defRPr sz="1000" b="1"/>
       </a:pPr>
-      <a:endParaRPr lang="de-DE"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3365,6 +3991,18 @@
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="15">
   <a:schemeClr val="accent2"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
+  <a:schemeClr val="accent6"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
+  <a:schemeClr val="accent6"/>
 </cs:colorStyle>
 </file>
 
@@ -3919,6 +4557,1012 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style10.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -7957,6 +9601,80 @@
       <xdr:colOff>219075</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing10.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2342008</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>447676</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>144780</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>171068</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8245,18 +9963,18 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>447676</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>2362200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>292228</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>171068</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -8566,16 +10284,16 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>52</v>
       </c>
@@ -8590,7 +10308,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8598,7 +10316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>53</v>
       </c>
@@ -8606,7 +10324,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>56</v>
       </c>
@@ -8614,7 +10332,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>54</v>
       </c>
@@ -8622,7 +10340,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>55</v>
       </c>
@@ -8630,7 +10348,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>57</v>
       </c>
@@ -8638,7 +10356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>59</v>
       </c>
@@ -8646,7 +10364,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>58</v>
       </c>
@@ -8654,7 +10372,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>60</v>
       </c>
@@ -8662,38 +10380,349 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+    </row>
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="C11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="C12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="C19" s="1"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8713,13 +10742,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>64</v>
       </c>
@@ -8734,7 +10763,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8742,7 +10771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>65</v>
       </c>
@@ -8750,7 +10779,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>67</v>
       </c>
@@ -8758,7 +10787,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>66</v>
       </c>
@@ -8766,7 +10795,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>68</v>
       </c>
@@ -8774,49 +10803,49 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
@@ -8837,14 +10866,14 @@
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="52.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>75</v>
       </c>
@@ -8860,7 +10889,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -8871,7 +10900,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
@@ -8882,7 +10911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -8893,7 +10922,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>51</v>
       </c>
@@ -8901,7 +10930,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -8912,7 +10941,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -8923,7 +10952,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
@@ -8934,7 +10963,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>14</v>
       </c>
@@ -8945,7 +10974,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
@@ -8956,7 +10985,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -8967,7 +10996,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>36</v>
       </c>
@@ -8978,7 +11007,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>12</v>
       </c>
@@ -8989,7 +11018,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>24</v>
       </c>
@@ -9000,7 +11029,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>27</v>
       </c>
@@ -9011,7 +11040,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -9022,7 +11051,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -9033,7 +11062,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
@@ -9044,7 +11073,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>22</v>
       </c>
@@ -9055,7 +11084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -9066,7 +11095,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>61</v>
       </c>
@@ -9077,7 +11106,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>41</v>
       </c>
@@ -9085,34 +11114,34 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="3"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="3"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="3"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="3"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="3"/>
     </row>
   </sheetData>
@@ -9133,14 +11162,14 @@
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>76</v>
       </c>
@@ -9156,7 +11185,7 @@
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
     </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9167,7 +11196,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -9178,7 +11207,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
@@ -9186,7 +11215,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
@@ -9194,7 +11223,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>38</v>
       </c>
@@ -9205,7 +11234,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>43</v>
       </c>
@@ -9213,7 +11242,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>37</v>
       </c>
@@ -9221,7 +11250,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>63</v>
       </c>
@@ -9232,7 +11261,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>45</v>
       </c>
@@ -9240,7 +11269,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>62</v>
       </c>
@@ -9248,7 +11277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>47</v>
       </c>
@@ -9256,7 +11285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -9264,7 +11293,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>0</v>
       </c>
@@ -9272,26 +11301,26 @@
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
       <c r="C20" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
     </row>
   </sheetData>
@@ -9315,13 +11344,13 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -9336,7 +11365,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9344,7 +11373,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -9352,7 +11381,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>72</v>
       </c>
@@ -9360,7 +11389,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>73</v>
       </c>
@@ -9368,7 +11397,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>70</v>
       </c>
@@ -9376,7 +11405,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>74</v>
       </c>
@@ -9384,46 +11413,46 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
@@ -9444,14 +11473,14 @@
       <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>69</v>
       </c>
@@ -9466,7 +11495,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9474,7 +11503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -9482,7 +11511,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -9490,7 +11519,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -9498,7 +11527,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>84</v>
       </c>
@@ -9506,7 +11535,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -9514,7 +11543,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -9522,7 +11551,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -9530,7 +11559,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>89</v>
       </c>
@@ -9538,7 +11567,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>82</v>
       </c>
@@ -9546,7 +11575,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>90</v>
       </c>
@@ -9554,7 +11583,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>81</v>
       </c>
@@ -9562,7 +11591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>80</v>
       </c>
@@ -9570,7 +11599,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -9578,22 +11607,22 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
@@ -9617,13 +11646,13 @@
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>96</v>
       </c>
@@ -9638,7 +11667,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9646,7 +11675,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>92</v>
       </c>
@@ -9654,7 +11683,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>93</v>
       </c>
@@ -9662,7 +11691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>94</v>
       </c>
@@ -9670,7 +11699,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>95</v>
       </c>
@@ -9678,7 +11707,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>91</v>
       </c>
@@ -9686,46 +11715,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
@@ -9743,16 +11772,16 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>97</v>
       </c>
@@ -9767,7 +11796,7 @@
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -9775,7 +11804,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>98</v>
       </c>
@@ -9783,7 +11812,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>99</v>
       </c>
@@ -9791,7 +11820,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>100</v>
       </c>
@@ -9799,7 +11828,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>102</v>
       </c>
@@ -9807,7 +11836,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>101</v>
       </c>
@@ -9815,46 +11844,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="4"/>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="4"/>
     </row>
   </sheetData>
@@ -9869,173 +11898,123 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="6"/>
-    </row>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B6">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>11</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <v>3</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>3</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
-      <c r="C15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
-      <c r="C16" s="1"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
-      <c r="C17" s="1"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
-      <c r="C21" s="1"/>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>